<commit_message>
arrange todo list on 2013-02-14.
</commit_message>
<xml_diff>
--- a/PdfPub/trunk/docs/mcs1-todo.xlsx
+++ b/PdfPub/trunk/docs/mcs1-todo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>●SakuttoBook/MCS　TODOリスト</t>
     <phoneticPr fontId="1"/>
@@ -434,6 +434,21 @@
     </rPh>
     <rPh sb="27" eb="28">
       <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>めくりの方向を、pdfDefine.csvで指定できるようにする</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シミュレータの機種変更時に、CSVも消してコピーしなおす。（初回起動時と同じにする）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>改善</t>
+    <rPh sb="0" eb="2">
+      <t>カイゼン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -477,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,6 +502,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,7 +573,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -602,8 +623,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -616,17 +645,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="57">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -651,6 +686,10 @@
     <cellStyle name="ハイパーリンク" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -676,6 +715,10 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="56" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1007,7 +1050,7 @@
   <dimension ref="B2:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1023,7 +1066,7 @@
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2"/>
@@ -1031,494 +1074,502 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="11">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="11">
+      <c r="B5" s="13">
+        <v>50</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="8"/>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="8"/>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="8"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="8">
+        <v>4</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="8"/>
+      <c r="C13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="8"/>
+      <c r="C14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="8"/>
+      <c r="C15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="8"/>
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="8">
+        <v>5</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="11"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="6" t="s">
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="11"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6" t="s">
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="8"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="11"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="11"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6" t="s">
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="8"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="8"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="11"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="6" t="s">
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="8"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="11"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="6" t="s">
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="8"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="11"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="6" t="s">
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="8"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="11"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="6" t="s">
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="8"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="11"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="6" t="s">
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="8"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="11"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="11"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="11"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="11"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="11"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="11"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="11"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="11">
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="8"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="8"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="8"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="8"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="8">
         <v>3</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C31" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="11"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="6" t="s">
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="8"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="11"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="6" t="s">
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="8"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="11"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="6" t="s">
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="8"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="11"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="6" t="s">
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="8"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="11"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="6" t="s">
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="8"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="11"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="6" t="s">
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="8"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="11"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="6" t="s">
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="8"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="11">
-        <v>2</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="11"/>
-      <c r="C31" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="11"/>
-      <c r="C32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="11">
-        <v>4</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="11"/>
-      <c r="C34" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="11"/>
-      <c r="C35" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="11"/>
-      <c r="C36" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="11"/>
-      <c r="C37" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="11"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
+      <c r="E38" s="11"/>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="11"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="11"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="11"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="11">
-        <v>5</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="11">
+      <c r="B43" s="8">
+        <v>6</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="8">
         <v>11</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C44" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="11"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="11"/>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="11">
-        <v>25</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="11"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="10"/>
+      <c r="B46" s="8">
+        <v>25</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11"/>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="11">
-        <v>18</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="7"/>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="11">
+      <c r="B48" s="8">
+        <v>18</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" s="8">
         <v>21</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C49" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="11"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
     </row>
     <row r="50" spans="2:5">
-      <c r="B50" s="11"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="10"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="2:5">
-      <c r="B51" s="11"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="2:5">
-      <c r="B52" s="11"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="2:5">
-      <c r="B53" s="11"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="10"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="2:5">
-      <c r="B54" s="11"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="10"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" spans="2:5">
-      <c r="B55" s="11">
-        <v>20</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="5"/>
       <c r="D55" s="6"/>
       <c r="E55" s="7"/>
     </row>
     <row r="56" spans="2:5">
-      <c r="B56" s="11">
-        <v>50</v>
-      </c>
-      <c r="C56" s="5" t="s">
+      <c r="B56" s="8">
+        <v>20</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="10"/>
+      <c r="E56" s="11"/>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="8"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="8"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="7"/>
+    </row>
+    <row r="59" spans="2:5" ht="52" customHeight="1">
+      <c r="B59" s="8">
         <v>30</v>
       </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="7"/>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" s="11"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="10"/>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="B58" s="11"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="10"/>
-    </row>
-    <row r="59" spans="2:5" ht="52" customHeight="1">
-      <c r="B59" s="11">
-        <v>30</v>
-      </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="7"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D40:E40"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arrange TODO list on 2013-03-01 from Kamikouchi.
</commit_message>
<xml_diff>
--- a/PdfPub/trunk/docs/mcs1-todo.xlsx
+++ b/PdfPub/trunk/docs/mcs1-todo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>●SakuttoBook/MCS　TODOリスト</t>
     <phoneticPr fontId="1"/>
@@ -434,6 +434,165 @@
     </rPh>
     <rPh sb="27" eb="28">
       <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>英語表記に対応</t>
+    <rPh sb="0" eb="4">
+      <t>エイゴヒョウキ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PDFビューアの下に、広告を入れられるようにする</t>
+    <rPh sb="8" eb="9">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>コウコク</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>iPhone5用のPDFを入れられるようにする</t>
+    <rPh sb="7" eb="8">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3/1上高地さんから</t>
+    <rPh sb="3" eb="6">
+      <t>カミコウチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実機にインストールした際に、動画があると、いくつも入ってしまう。メモリも圧迫する（？）</t>
+    <rPh sb="0" eb="2">
+      <t>ジッキ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ドウガ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>アッパク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ページの位置を示すスライダをつける</t>
+    <rPh sb="4" eb="6">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>シメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>URLリンクをタップした際に、今は何で開くか選択肢が出るが、選択肢を出さずに常に内部ビューアで開く（URLを表示しないため、隠しページに誘導できる）</t>
+    <rPh sb="12" eb="13">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>イマ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="22" eb="25">
+      <t>センタクシ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="30" eb="33">
+      <t>センタクシ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ツネ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ユウドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>製品ラインナップの整理。Lite版、通常版、Pro版と分ける。</t>
+    <rPh sb="0" eb="2">
+      <t>セイヒン</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>セイリ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t>ツウジョウバン</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>くまがい印刷さん、CSVファイルに_1が付いたままでzipにしていた。。。zipを展開してコピーする時には先頭一致で探すモードをつけるべきかも。</t>
+    <rPh sb="4" eb="6">
+      <t>インサツ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ツ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>テンカイ</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="53" eb="57">
+      <t>セントウイッチ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>サガ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -552,7 +711,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -602,8 +761,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -616,17 +789,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="56" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="63">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -651,6 +825,13 @@
     <cellStyle name="ハイパーリンク" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -676,6 +857,13 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="62" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1004,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E59"/>
+  <dimension ref="B2:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1023,7 +1211,7 @@
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2"/>
@@ -1031,454 +1219,580 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="11"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="6" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="11"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="11"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="11"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="11"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="6" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="11"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="11"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="6" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="11"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="11"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="6" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="11"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="11"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="11"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="11"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="11"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="11"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="11"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="11">
+      <c r="B22" s="8">
         <v>3</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="11"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="6" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="11"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="6" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="11"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="6" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="11"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="6" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="11"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="6" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="11"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="6" t="s">
+      <c r="B28" s="8"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="7"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="11"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="6" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="11">
+      <c r="B30" s="8">
         <v>2</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="11"/>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="11"/>
-      <c r="C32" s="8" t="s">
+      <c r="B32" s="8"/>
+      <c r="C32" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="11">
+      <c r="B33" s="8">
         <v>4</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="11"/>
-      <c r="C34" s="8" t="s">
+      <c r="B34" s="8"/>
+      <c r="C34" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="11"/>
-      <c r="C35" s="8" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="7"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="11"/>
-      <c r="C36" s="8" t="s">
+      <c r="B36" s="8"/>
+      <c r="C36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="7"/>
+      <c r="E36" s="11"/>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="11"/>
-      <c r="C37" s="8" t="s">
+      <c r="B37" s="8"/>
+      <c r="C37" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="7"/>
+      <c r="E37" s="11"/>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="11"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11"/>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="11"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="11"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="11"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="11">
+      <c r="B42" s="8">
         <v>5</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="11">
+      <c r="B43" s="8">
         <v>11</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="11"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="11">
+      <c r="B45" s="8">
         <v>25</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="7"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="11"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="10"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="11">
+      <c r="B47" s="8">
         <v>18</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="11">
+      <c r="B48" s="8">
         <v>21</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
     </row>
     <row r="49" spans="2:5">
-      <c r="B49" s="11"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="10"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="2:5">
-      <c r="B50" s="11"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="10"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="2:5">
-      <c r="B51" s="11"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="2:5">
-      <c r="B52" s="11"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="2:5">
-      <c r="B53" s="11"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="10"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="2:5">
-      <c r="B54" s="11"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="10"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" spans="2:5">
-      <c r="B55" s="11">
+      <c r="B55" s="8">
         <v>20</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="7"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="11"/>
     </row>
     <row r="56" spans="2:5">
-      <c r="B56" s="11">
+      <c r="B56" s="8">
         <v>50</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="7"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="11"/>
     </row>
     <row r="57" spans="2:5">
-      <c r="B57" s="11"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="10"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="2:5">
-      <c r="B58" s="11"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="10"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" spans="2:5" ht="52" customHeight="1">
-      <c r="B59" s="11">
+      <c r="B59" s="8">
         <v>30</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="7"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="11"/>
+    </row>
+    <row r="60" spans="2:5">
+      <c r="B60" s="8"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="11"/>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" s="10"/>
+      <c r="E61" s="11"/>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11"/>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="10"/>
+      <c r="E63" s="11"/>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="B64" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="10"/>
+      <c r="E64" s="11"/>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" s="10"/>
+      <c r="E65" s="11"/>
+    </row>
+    <row r="66" spans="2:5" ht="32" customHeight="1">
+      <c r="B66" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="11"/>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="8"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="11"/>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="10"/>
+      <c r="E68" s="11"/>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="8"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="11"/>
+    </row>
+    <row r="70" spans="2:5" ht="46" customHeight="1">
+      <c r="B70" s="8"/>
+      <c r="C70" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="10"/>
+      <c r="E70" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
+  <mergeCells count="56">
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C55:E55"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
@@ -1495,30 +1809,11 @@
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arrange TODO on 2013-03-11.
</commit_message>
<xml_diff>
--- a/PdfPub/trunk/docs/mcs1-todo.xlsx
+++ b/PdfPub/trunk/docs/mcs1-todo.xlsx
@@ -19,13 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>●SakuttoBook/MCS　TODOリスト</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・URLリンクを、CSVファイルで指定できるようにする。</t>
   </si>
   <si>
     <t>・音声停止ボタンを、まったく表示しないように切り替える設定を追加する</t>
@@ -164,16 +161,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ジャンルをContentListDSの各コンテンツに含める。</t>
-    <rPh sb="19" eb="20">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="26" eb="27">
-      <t>フク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>親コンテンツIDをContentListDSの各コンテンツに含める。</t>
     <rPh sb="0" eb="1">
       <t>オヤ</t>
@@ -238,28 +225,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>zip ファイルのダウンロード用リンクも変わるので、対応。</t>
-    <rPh sb="15" eb="16">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>タイオウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>v2</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>v2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>v1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -299,145 +269,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>定数の定義は、define.h から、define_const.hか何かに移す。</t>
-    <rPh sb="0" eb="2">
-      <t>テイスウ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>テイギ</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>ウツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「ePubs.jp store」として、リリースする</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>アイコンを、ホームページロゴから作成</t>
-    <rPh sb="16" eb="18">
-      <t>サクセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ジャンルに分けるため、TabViewを入れる</t>
-    <rPh sb="5" eb="6">
-      <t>ワ</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>イ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>コンテンツ一覧を、サーバの内容で上書きしない設定に。</t>
-    <rPh sb="5" eb="7">
-      <t>イチラン</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>ウワガ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>AppIDの取得。epubsjpstore</t>
-    <rPh sb="6" eb="8">
-      <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>コンテンツをサーバに登録。祖父の従軍日記、旧聞日本橋、DiviDeco Hair、同動画</t>
-    <rPh sb="10" eb="12">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ソフ</t>
-    </rPh>
-    <rPh sb="16" eb="20">
-      <t>ジュウグンニッキ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>キュウブン</t>
-    </rPh>
-    <rPh sb="23" eb="26">
-      <t>ニホンバシ</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ドウ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ドウガ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>コンテンツの準備ーDiviDeco Hair、同画像</t>
-    <rPh sb="6" eb="8">
-      <t>ジュンビ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>ドウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ガゾウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>コンテンツの準備ー祖父の従軍日記。Wordに入れて、PDF化。</t>
-    <rPh sb="6" eb="8">
-      <t>ジュンビ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ソフ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ジュウグン</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ニッキ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>カ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>コンテンツの準備ー旧聞日本橋。Wordに入れて、PDF化。</t>
-    <rPh sb="6" eb="8">
-      <t>ジュンビ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>キュウブン</t>
-    </rPh>
-    <rPh sb="11" eb="14">
-      <t>ニホンバシ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>カ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>英語表記に対応</t>
     <rPh sb="0" eb="4">
       <t>エイゴヒョウキ</t>
@@ -612,6 +443,19 @@
     </rPh>
     <rPh sb="18" eb="20">
       <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>上部のメニューバーをBlackにしたい。（プログラム上で変更できないか）</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウブ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ヘンコウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -730,8 +574,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -821,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="77">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -854,6 +710,12 @@
     <cellStyle name="ハイパーリンク" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -887,6 +749,12 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="76" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1215,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E71"/>
+  <dimension ref="B2:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71:E71"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1235,617 +1103,422 @@
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>1</v>
-      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="8">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="8"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="B6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="13"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="8"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="B7" s="8">
+        <v>25</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="8"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="8">
+        <v>21</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="8"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="D9" s="12"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="8"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="12"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="8"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="12" t="s">
-        <v>36</v>
-      </c>
+      <c r="B13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="8"/>
       <c r="C14" s="5"/>
       <c r="D14" s="12" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="8"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="8"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="8"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="E17" s="13"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="8"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="8"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="8"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="8"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="8">
+        <v>2</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="D21" s="12"/>
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="8">
-        <v>3</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="12"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="8"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="B23" s="8">
+        <v>4</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="12"/>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="8"/>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="D24" s="12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="8"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="D25" s="12" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="8"/>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D26" s="12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="D27" s="12"/>
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="8"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="8"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="13"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="8">
-        <v>2</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="8"/>
-      <c r="C31" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="B31" s="8">
+        <v>5</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="13"/>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="8"/>
-      <c r="C32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="B32" s="8">
+        <v>11</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="12"/>
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="8">
-        <v>4</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="8"/>
-      <c r="C34" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="13"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="8"/>
-      <c r="C35" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="B35" s="8">
+        <v>18</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="12"/>
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="8"/>
-      <c r="C36" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="13"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="8"/>
-      <c r="C37" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="8"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="D38" s="12"/>
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="8"/>
-      <c r="C39" s="5"/>
+      <c r="B39" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13"/>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="8"/>
-      <c r="C40" s="5"/>
+      <c r="B40" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="D40" s="12"/>
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="8"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="8">
-        <v>5</v>
+      <c r="B41" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="13"/>
+    </row>
+    <row r="42" spans="2:5" ht="32" customHeight="1">
+      <c r="B42" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="8">
-        <v>11</v>
-      </c>
+      <c r="B43" s="8"/>
       <c r="C43" s="11" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="13"/>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="8"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
+      <c r="B44" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="13"/>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="8">
-        <v>25</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>6</v>
-      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="12"/>
       <c r="E45" s="13"/>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="2:5" ht="46" customHeight="1">
       <c r="B46" s="8"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="2:5">
+      <c r="C46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="13"/>
+    </row>
+    <row r="47" spans="2:5" ht="52" customHeight="1">
       <c r="B47" s="8">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="13"/>
     </row>
-    <row r="48" spans="2:5">
-      <c r="B48" s="8">
-        <v>21</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="13"/>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="8"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="7"/>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="8"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="51" spans="2:5">
-      <c r="B51" s="8"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="8"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="7"/>
-    </row>
-    <row r="53" spans="2:5">
-      <c r="B53" s="8"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="7"/>
-    </row>
-    <row r="54" spans="2:5">
-      <c r="B54" s="8"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="7"/>
-    </row>
-    <row r="55" spans="2:5">
-      <c r="B55" s="8">
-        <v>20</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="13"/>
-    </row>
-    <row r="56" spans="2:5">
-      <c r="B56" s="8">
-        <v>50</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="13"/>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" s="8"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="7"/>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="B58" s="8"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="7"/>
-    </row>
-    <row r="59" spans="2:5" ht="52" customHeight="1">
-      <c r="B59" s="8">
-        <v>30</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="13"/>
-    </row>
-    <row r="60" spans="2:5">
-      <c r="B60" s="8"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="13"/>
-    </row>
-    <row r="61" spans="2:5">
-      <c r="B61" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D61" s="12"/>
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" spans="2:5">
-      <c r="B62" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="13"/>
-    </row>
-    <row r="63" spans="2:5">
-      <c r="B63" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D63" s="12"/>
-      <c r="E63" s="13"/>
-    </row>
-    <row r="64" spans="2:5">
-      <c r="B64" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D64" s="12"/>
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" spans="2:5">
-      <c r="B65" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="13"/>
-    </row>
-    <row r="66" spans="2:5" ht="32" customHeight="1">
-      <c r="B66" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D66" s="12"/>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="2:5">
-      <c r="B67" s="8"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="13"/>
-    </row>
-    <row r="68" spans="2:5">
-      <c r="B68" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="13"/>
-    </row>
-    <row r="69" spans="2:5">
-      <c r="B69" s="8"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="13"/>
-    </row>
-    <row r="70" spans="2:5" ht="46" customHeight="1">
-      <c r="B70" s="8"/>
-      <c r="C70" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D70" s="12"/>
-      <c r="E70" s="13"/>
-    </row>
-    <row r="71" spans="2:5">
-      <c r="B71" s="8"/>
-      <c r="C71" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D71" s="12"/>
-      <c r="E71" s="13"/>
-    </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D19:E19"/>
+  <mergeCells count="40">
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="C47:E47"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D20:E20"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arrange TODO at 2013-03-12.
</commit_message>
<xml_diff>
--- a/PdfPub/trunk/docs/mcs1-todo.xlsx
+++ b/PdfPub/trunk/docs/mcs1-todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>●SakuttoBook/MCS　TODOリスト</t>
     <phoneticPr fontId="1"/>
@@ -466,6 +466,13 @@
     </rPh>
     <rPh sb="32" eb="33">
       <t>ケ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>マーカーペンを追加(JPPBookのソースから)</t>
+    <rPh sb="7" eb="9">
+      <t>ツイカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -584,8 +591,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -691,7 +700,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="83">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -732,6 +741,7 @@
     <cellStyle name="ハイパーリンク" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -773,6 +783,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="82" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1101,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E47"/>
+  <dimension ref="B2:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1139,61 +1150,65 @@
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="8">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="10" t="s">
-        <v>29</v>
+      <c r="B6" s="8">
+        <v>20</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="8">
-        <v>25</v>
+      <c r="B7" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="8">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="8"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="8">
+        <v>21</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="8"/>
-      <c r="C10" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" s="12"/>
       <c r="E11" s="13"/>
     </row>
@@ -1204,28 +1219,26 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="8">
-        <v>3</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>7</v>
-      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="8"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="8"/>
       <c r="C15" s="5"/>
       <c r="D15" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="13"/>
     </row>
@@ -1233,7 +1246,7 @@
       <c r="B16" s="8"/>
       <c r="C16" s="5"/>
       <c r="D16" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="13"/>
     </row>
@@ -1241,7 +1254,7 @@
       <c r="B17" s="8"/>
       <c r="C17" s="5"/>
       <c r="D17" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="13"/>
     </row>
@@ -1249,7 +1262,7 @@
       <c r="B18" s="8"/>
       <c r="C18" s="5"/>
       <c r="D18" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="13"/>
     </row>
@@ -1257,7 +1270,7 @@
       <c r="B19" s="8"/>
       <c r="C19" s="5"/>
       <c r="D19" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="13"/>
     </row>
@@ -1265,48 +1278,46 @@
       <c r="B20" s="8"/>
       <c r="C20" s="5"/>
       <c r="D20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="8"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="8">
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="8">
         <v>2</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="8"/>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="8"/>
+      <c r="C23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="8">
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="8">
         <v>4</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="8"/>
-      <c r="C24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="D24" s="12"/>
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5">
@@ -1315,24 +1326,28 @@
         <v>21</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="8"/>
       <c r="C26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="8"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="12"/>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5">
@@ -1350,34 +1365,34 @@
     <row r="30" spans="2:5">
       <c r="B30" s="8"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="8">
-        <v>5</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="8">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="8"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
+      <c r="B33" s="8">
+        <v>11</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="8"/>
@@ -1386,34 +1401,30 @@
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="8">
+      <c r="B35" s="8"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="8">
         <v>18</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="8"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="8"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="13"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="12"/>
       <c r="E38" s="13"/>
     </row>
@@ -1422,7 +1433,7 @@
         <v>29</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13"/>
@@ -1432,7 +1443,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="13"/>
@@ -1442,105 +1453,116 @@
         <v>29</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="13"/>
     </row>
-    <row r="42" spans="2:5" ht="32" customHeight="1">
+    <row r="42" spans="2:5">
       <c r="B42" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
     </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="8"/>
+    <row r="43" spans="2:5" ht="32" customHeight="1">
+      <c r="B43" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="C43" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="13"/>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="10" t="s">
-        <v>29</v>
-      </c>
+      <c r="B44" s="8"/>
       <c r="C44" s="11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="13"/>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="8"/>
-      <c r="C45" s="11"/>
+      <c r="B45" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="D45" s="12"/>
       <c r="E45" s="13"/>
     </row>
-    <row r="46" spans="2:5" ht="46" customHeight="1">
+    <row r="46" spans="2:5">
       <c r="B46" s="8"/>
-      <c r="C46" s="11" t="s">
-        <v>34</v>
-      </c>
+      <c r="C46" s="11"/>
       <c r="D46" s="12"/>
       <c r="E46" s="13"/>
     </row>
-    <row r="47" spans="2:5" ht="52" customHeight="1">
-      <c r="B47" s="8">
-        <v>30</v>
-      </c>
+    <row r="47" spans="2:5" ht="46" customHeight="1">
+      <c r="B47" s="8"/>
       <c r="C47" s="11" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="13"/>
     </row>
+    <row r="48" spans="2:5" ht="52" customHeight="1">
+      <c r="B48" s="8">
+        <v>30</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
+    <mergeCell ref="C42:E42"/>
     <mergeCell ref="C47:E47"/>
-    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C48:E48"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="C39:E39"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C35:E35"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update TODO at 2013-03-15.
</commit_message>
<xml_diff>
--- a/PdfPub/trunk/docs/mcs1-todo.xlsx
+++ b/PdfPub/trunk/docs/mcs1-todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>●SakuttoBook/MCS　TODOリスト</t>
     <phoneticPr fontId="1"/>
@@ -508,6 +508,49 @@
     <rPh sb="86" eb="89">
       <t>ヒヒョウジ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Define.hでリストアボタンを非表示にすることは可能でしょうか。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3/13 上高地さんから</t>
+    <rPh sb="5" eb="8">
+      <t>カミコウチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・iPhone5用のCSVファイルを使えるようにする。接尾辞は「-iphone5」。</t>
+    <rPh sb="8" eb="9">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>iPhone版で、マーカーを全削除する際に、「キャンセル」と「Cancel」とボタンが２つ表示される</t>
+    <rPh sb="6" eb="7">
+      <t>バン</t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t>ゼンサクジョ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリ内課金を使用してアプリ内課金を使わずに、組み込みコンテンツだけにす 
+る場合、リストアボタンが表示されために、リジェクトされるようです
+Define.hでリストアボタンを非表示にすることは可能でしょうか。</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -550,7 +593,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +603,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,7 +674,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -717,8 +766,98 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -741,8 +880,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="56" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="181">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -788,6 +934,51 @@
     <cellStyle name="ハイパーリンク" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -834,6 +1025,51 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="180" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1164,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50:E50"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1199,104 +1435,106 @@
       <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="8">
+      <c r="B5" s="14">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="8">
-        <v>20</v>
-      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="11" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="10" t="s">
-        <v>29</v>
+      <c r="B7" s="8">
+        <v>20</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="8">
-        <v>25</v>
+      <c r="B8" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="8">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="8"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="8">
+        <v>21</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="8"/>
-      <c r="C11" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="C11" s="5"/>
       <c r="D11" s="12"/>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="8"/>
-      <c r="C12" s="5"/>
+      <c r="C12" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="8">
-        <v>3</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>7</v>
-      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="8"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="12"/>
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="8"/>
       <c r="C16" s="5"/>
       <c r="D16" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="13"/>
     </row>
@@ -1304,7 +1542,7 @@
       <c r="B17" s="8"/>
       <c r="C17" s="5"/>
       <c r="D17" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="13"/>
     </row>
@@ -1312,7 +1550,7 @@
       <c r="B18" s="8"/>
       <c r="C18" s="5"/>
       <c r="D18" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="13"/>
     </row>
@@ -1320,7 +1558,7 @@
       <c r="B19" s="8"/>
       <c r="C19" s="5"/>
       <c r="D19" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="13"/>
     </row>
@@ -1328,7 +1566,7 @@
       <c r="B20" s="8"/>
       <c r="C20" s="5"/>
       <c r="D20" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="13"/>
     </row>
@@ -1336,48 +1574,46 @@
       <c r="B21" s="8"/>
       <c r="C21" s="5"/>
       <c r="D21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="8"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="8">
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="8">
         <v>2</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="8"/>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="8"/>
+      <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D24" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="8">
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="8">
         <v>4</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="8"/>
-      <c r="C25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="D25" s="12"/>
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5">
@@ -1386,24 +1622,28 @@
         <v>21</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="8"/>
       <c r="C27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="8"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="12"/>
+      <c r="C28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="2:5">
@@ -1418,11 +1658,13 @@
       <c r="D30" s="12"/>
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" ht="52" customHeight="1">
       <c r="B31" s="8"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
+      <c r="C31" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="8">
@@ -1499,14 +1741,14 @@
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="13"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="17"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="10" t="s">
@@ -1547,8 +1789,12 @@
       <c r="E45" s="13"/>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="8"/>
-      <c r="C46" s="11"/>
+      <c r="B46" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="D46" s="12"/>
       <c r="E46" s="13"/>
     </row>
@@ -1585,37 +1831,10 @@
       <c r="E50" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="C5:E5"/>
+  <mergeCells count="44">
     <mergeCell ref="C42:E42"/>
     <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="C45:E45"/>
@@ -1623,12 +1842,40 @@
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arrange TODO at 2013-03-20.
</commit_message>
<xml_diff>
--- a/PdfPub/trunk/docs/mcs1-todo.xlsx
+++ b/PdfPub/trunk/docs/mcs1-todo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500"/>
@@ -875,18 +875,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="56" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="56" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="56" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="181">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1400,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48:E48"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1428,263 +1428,263 @@
       <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="8"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="8">
         <v>20</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="8">
+      <c r="B9" s="11">
         <v>25</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="8">
         <v>21</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="8"/>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="8"/>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="8"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="8">
         <v>3</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="8"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="8"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="8"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="8"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="8"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="13"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="8"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="13"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="8">
         <v>2</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="8"/>
       <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="13"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="8">
         <v>4</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="8"/>
       <c r="C26" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="13"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="8"/>
       <c r="C27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="13"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="8"/>
       <c r="C28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="8"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="8"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" spans="2:5" ht="52" customHeight="1">
-      <c r="B31" s="8"/>
-      <c r="C31" s="11" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="8">
         <v>5</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="15"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="8">
         <v>11</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="8"/>
@@ -1702,11 +1702,11 @@
       <c r="B36" s="8">
         <v>18</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="8"/>
@@ -1716,122 +1716,150 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="8"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="15"/>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="13"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="15"/>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="15"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="16"/>
-      <c r="E41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="15"/>
     </row>
     <row r="43" spans="2:5" ht="32" customHeight="1">
       <c r="B43" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="15"/>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="8"/>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="13"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="15"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="13"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="2:5" ht="46" customHeight="1">
       <c r="B47" s="8"/>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="15"/>
     </row>
     <row r="48" spans="2:5" ht="52" customHeight="1">
       <c r="B48" s="8">
         <v>30</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="13"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="15"/>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="8"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="2:5" ht="36" customHeight="1">
       <c r="B50" s="8"/>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="13"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C31:E31"/>
     <mergeCell ref="C42:E42"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C8:E8"/>
@@ -1848,34 +1876,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arrange TODO list on 2013-05-01.(move to "Issues" in github.)
</commit_message>
<xml_diff>
--- a/PdfPub/trunk/docs/mcs1-todo.xlsx
+++ b/PdfPub/trunk/docs/mcs1-todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>●SakuttoBook/MCS　TODOリスト</t>
     <phoneticPr fontId="1"/>
@@ -551,6 +551,13 @@
     <t>アプリ内課金を使用してアプリ内課金を使わずに、組み込みコンテンツだけにす 
 る場合、リストアボタンが表示されために、リジェクトされるようです
 Define.hでリストアボタンを非表示にすることは可能でしょうか。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-&gt;github の Issues に移行した。</t>
+    <rPh sb="20" eb="22">
+      <t>イコウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -558,7 +565,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -589,6 +596,14 @@
       <color theme="11"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -857,7 +872,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -887,6 +902,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="181">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1400,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1415,6 +1431,9 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="E2" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="9" t="s">
@@ -1832,6 +1851,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C31:E31"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="C48:E48"/>
@@ -1848,34 +1895,6 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="C25:E25"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>